<commit_message>
Added UpdateItemPrice Column in Import / export sheet for Catalog page.[TF00287]
</commit_message>
<xml_diff>
--- a/pur/catalog/usr/ItemsTemplate.xlsx
+++ b/pur/catalog/usr/ItemsTemplate.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Deepa\Dropbox (i3)\repos\js\crothall\js-crothall-chimes-fin-trans\pur\catalog\usr\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="270" yWindow="-30" windowWidth="15480" windowHeight="7095"/>
   </bookViews>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Active</t>
   </si>
@@ -36,16 +41,19 @@
   <si>
     <t>CatalogTitle</t>
   </si>
+  <si>
+    <t>UpdateItemPrice</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
     <numFmt numFmtId="165" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,6 +634,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -672,7 +688,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -704,9 +720,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -738,6 +755,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -913,14 +931,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" style="9" customWidth="1"/>
@@ -943,7 +961,7 @@
     <col min="21" max="21" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1">
+    <row r="1" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -962,7 +980,9 @@
       <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="10"/>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="14"/>

</xml_diff>